<commit_message>
7.10 Fixed Some Bugs
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/2_Canteen.xlsx
+++ b/Assets/StreamingAssets/2_Canteen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C53D4F-8669-BD4E-AFB0-19ECA5E175B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23D50DC-A8D9-C84D-A11B-3D85135954E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="540" windowWidth="28100" windowHeight="15820" xr2:uid="{68C9ECD6-F2C7-A34A-8665-FFA8663C762C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -328,27 +328,6 @@
   <si>
     <t>???</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Room-Outside3</t>
-  </si>
-  <si>
-    <t>Room-Outside4</t>
-  </si>
-  <si>
-    <t>Room-Outside5</t>
-  </si>
-  <si>
-    <t>Room-Outside6</t>
-  </si>
-  <si>
-    <t>Room-Outside7</t>
-  </si>
-  <si>
-    <t>Room-Outside8</t>
-  </si>
-  <si>
-    <t>Room-Outside9</t>
   </si>
   <si>
     <t>Sir...</t>
@@ -803,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EEC272-F350-D34D-A243-3179172F76FB}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -890,7 +869,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="34">
@@ -901,7 +880,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="17">
@@ -909,7 +888,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -918,7 +897,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>27</v>
@@ -953,7 +932,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -967,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -976,7 +955,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1005,7 +984,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1028,7 +1007,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>17</v>
@@ -1189,7 +1168,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -1220,7 +1199,7 @@
     </row>
     <row r="22" spans="1:12" ht="51">
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -1234,7 +1213,7 @@
     </row>
     <row r="23" spans="1:12" ht="51">
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
@@ -1251,7 +1230,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
@@ -1277,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1297,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
@@ -1317,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -1409,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
@@ -1528,7 +1507,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -1559,7 +1538,7 @@
     </row>
     <row r="40" spans="1:12" ht="34">
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
         <v>15</v>

</xml_diff>